<commit_message>
update defaults for experiments
</commit_message>
<xml_diff>
--- a/experiments/Measures.xlsx
+++ b/experiments/Measures.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rich\OneDrive\Python\Spotter-Amrron\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Spotter-Amrron\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F94C4AE-E8C6-4C71-8566-F2DABD92D882}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB71EC5-8E04-44FD-857B-1E16208934B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{3B2BA4DA-ED28-442C-94E4-7266A9A05D73}"/>
+    <workbookView minimized="1" xWindow="1905" yWindow="1320" windowWidth="16200" windowHeight="9360" activeTab="1" xr2:uid="{3B2BA4DA-ED28-442C-94E4-7266A9A05D73}"/>
   </bookViews>
   <sheets>
     <sheet name="Datastore" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="139">
   <si>
     <t>Data Element</t>
   </si>
@@ -455,6 +455,33 @@
   </si>
   <si>
     <t>Current Local</t>
+  </si>
+  <si>
+    <t>Base FLMsg (Spotv3)</t>
+  </si>
+  <si>
+    <t>Base FLMsg (sitrep)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current Weather: </t>
+  </si>
+  <si>
+    <t>24 hr Weather: (Temp;Rain;Wind)</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Grid</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -879,7 +906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B177603C-F232-40E2-A2EC-0009B5C24689}">
   <dimension ref="A1:R87"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C87" sqref="C71:C87"/>
     </sheetView>
   </sheetViews>
@@ -3520,125 +3547,161 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C66601F-92B0-41E4-88F1-C1E069D4B581}">
-  <dimension ref="B1:F19"/>
+  <dimension ref="B1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D3" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D5" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D6" s="9" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
+    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D7" s="11" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="9" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
+    <row r="9" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D9" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
+    <row r="10" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D10" s="11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D11" s="11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D12" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D13" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D14" s="11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D15" s="11" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
+    <row r="16" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D16" s="11" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
+    <row r="17" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D17" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
+    <row r="18" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D18" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D19" s="11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D20" s="11" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="11" t="s">
+    <row r="21" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D21" s="11" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="11" t="s">
+    <row r="22" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D22" s="11" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="11" t="s">
+    <row r="23" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D23" s="11" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="11" t="s">
+    <row r="24" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D24" s="11" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="11" t="s">
+    <row r="25" spans="4:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D25" s="11" t="s">
         <v>127</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1" xr:uid="{7B035AC0-413C-458D-B6F1-3B96D3A44519}"/>
+    <hyperlink ref="E1" r:id="rId1" xr:uid="{7B035AC0-413C-458D-B6F1-3B96D3A44519}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>